<commit_message>
added age pie chart
</commit_message>
<xml_diff>
--- a/analysis/data/lying_data.xlsx
+++ b/analysis/data/lying_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\School\2025\Spring 2025\INFO 698 - Capstone\GitHub Repo\misinformation-study\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265D01D1-80EE-44CD-BE10-36543E72C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44CA5A-6001-4FA2-8047-6D9AB8955E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9629" uniqueCount="1420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9629" uniqueCount="1446">
   <si>
     <t>GROUP</t>
   </si>
@@ -4347,6 +4347,84 @@
   </si>
   <si>
     <t>QQ1_WORD_COUNT_BEFORE</t>
+  </si>
+  <si>
+    <t>QQ1 2</t>
+  </si>
+  <si>
+    <t>QQ1_CHARACTER_COUNT3</t>
+  </si>
+  <si>
+    <t>QQ24</t>
+  </si>
+  <si>
+    <t>QQ2_CHARACTER_COUNT5</t>
+  </si>
+  <si>
+    <t>QQ36</t>
+  </si>
+  <si>
+    <t>QQ3_CHARACTER_COUNT7</t>
+  </si>
+  <si>
+    <t>First 10 Items _18</t>
+  </si>
+  <si>
+    <t>First 10 Items _29</t>
+  </si>
+  <si>
+    <t>First 10 Items _310</t>
+  </si>
+  <si>
+    <t>First 10 Items _411</t>
+  </si>
+  <si>
+    <t>First 10 Items _512</t>
+  </si>
+  <si>
+    <t>First 10 Items _613</t>
+  </si>
+  <si>
+    <t>First 10 Items _714</t>
+  </si>
+  <si>
+    <t>First 10 Items _815</t>
+  </si>
+  <si>
+    <t>First 10 Items _916</t>
+  </si>
+  <si>
+    <t>First 10 Items _1017</t>
+  </si>
+  <si>
+    <t>Last 10 Items _118</t>
+  </si>
+  <si>
+    <t>Last 10 Items _219</t>
+  </si>
+  <si>
+    <t>Last 10 Items _320</t>
+  </si>
+  <si>
+    <t>Last 10 Items _421</t>
+  </si>
+  <si>
+    <t>Last 10 Items _522</t>
+  </si>
+  <si>
+    <t>Last 10 Items _623</t>
+  </si>
+  <si>
+    <t>Last 10 Items _724</t>
+  </si>
+  <si>
+    <t>Last 10 Items _825</t>
+  </si>
+  <si>
+    <t>Last 10 Items _926</t>
+  </si>
+  <si>
+    <t>Last 10 Items _1027</t>
   </si>
 </sst>
 </file>
@@ -4815,7 +4893,2356 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="122">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAE2D5"/>
+          <bgColor rgb="FFFAE2D5"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4826,6 +7253,167 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C2C848D5-A266-46C6-A87A-C4B9154CB138}" name="Table1" displayName="Table1" ref="A1:DP101" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:DP101" xr:uid="{C2C848D5-A266-46C6-A87A-C4B9154CB138}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Control Group (Audio)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="120">
+    <tableColumn id="1" xr3:uid="{4BEAC8A5-9226-4BA2-91E7-14E9B47D3E09}" name="PARTICIPANT ID" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{EF4C3F5A-7852-4C02-8541-AEC12D919BF3}" name="GROUP" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{5AD7D02F-4433-4BB6-AB10-175ABD89725D}" name="Age" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{C3944AFF-CB17-4A39-B7B2-9AA8B7C0DF15}" name="Gender " dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{A672E2D8-B2B0-4BA8-BCEA-99F4B128B172}" name="Citizenship" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{8C6C4CF7-FD68-40C3-988F-97DABD2DD6B6}" name="Ethnicity" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{2745B3D0-02AF-4EAA-A4BD-D7F8C66A6852}" name="Ethnicity_6_TEXT" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{FFC7D8DF-54AF-4BFD-9F93-111C0A4C9AA9}" name="Religion" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{A8935703-B1F9-44EA-8D55-FEC093ED243E}" name="Religion_11_TEXT" dataDxfId="113"/>
+    <tableColumn id="10" xr3:uid="{F5EC22AC-F6C1-4F89-84BF-3AB7E60FF2C5}" name="Politics " dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{08077061-C415-4122-ADDB-4411B80422D4}" name="Politics _5_TEXT" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{046C78C3-B246-426E-825C-B67991456A64}" name="Platforms" dataDxfId="110"/>
+    <tableColumn id="13" xr3:uid="{1F5F6CB3-1C53-4D44-B093-875E28D7B87F}" name="Platforms_6_TEXT" dataDxfId="109"/>
+    <tableColumn id="14" xr3:uid="{8B0A6479-8F36-4D80-9467-2E6C877E9B36}" name="Time Spent " dataDxfId="108"/>
+    <tableColumn id="15" xr3:uid="{AA4C553D-9C80-4F2D-B566-432D3139CD6B}" name="Utility" dataDxfId="107"/>
+    <tableColumn id="16" xr3:uid="{52CAEF06-4684-4382-A692-689D053742B1}" name="Frequency" dataDxfId="106"/>
+    <tableColumn id="17" xr3:uid="{23133F51-3192-438A-BD8D-D404A0C88E76}" name="Top 3 Entertainment_1" dataDxfId="105"/>
+    <tableColumn id="18" xr3:uid="{32E5C7BE-7A81-4CC5-877B-2C6A5C699E25}" name="Top 3 Entertainment_2" dataDxfId="104"/>
+    <tableColumn id="19" xr3:uid="{179179B7-9860-4C35-9122-768E71B1C8BF}" name="Top 3 Entertainment_3" dataDxfId="103"/>
+    <tableColumn id="20" xr3:uid="{DC855606-9EE0-4366-A880-6410D2FE3C36}" name="Top 3 Educational _1" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{B37D843E-1665-43B4-9FDE-463B9202FA78}" name="Top 3 Educational _2" dataDxfId="101"/>
+    <tableColumn id="22" xr3:uid="{7AFF2AAD-C91D-42A8-A7CA-4AAFB4A31AA7}" name="Top 3 Educational _3" dataDxfId="100"/>
+    <tableColumn id="23" xr3:uid="{97679BA8-D60F-47B3-9D18-24E8B1591F63}" name="Ad-Free" dataDxfId="99"/>
+    <tableColumn id="24" xr3:uid="{0A168C1A-0CB2-4F81-A476-9D1DA064A3DB}" name="Ad Skipping " dataDxfId="98"/>
+    <tableColumn id="25" xr3:uid="{B0A972B6-2DF8-4C1F-AED4-97F270F0A97C}" name="Recommendation" dataDxfId="97"/>
+    <tableColumn id="26" xr3:uid="{5268196F-F2A5-4714-A739-3A125662C4EF}" name="QQ1 " dataDxfId="96"/>
+    <tableColumn id="27" xr3:uid="{AACD74D8-EC60-4B39-A24D-09BD8B5DB799}" name="QQ1_WORD_COUNT_BEFORE" dataDxfId="95">
+      <calculatedColumnFormula>IF(LEN(TRIM(Z2))=0, 0, LEN(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Z2, "/", " "), "-", " "), "  ", " "))) - LEN(SUBSTITUTE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(Z2, "/", " "), "-", " "), "  ", " ")), " ", "")) + 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="28" xr3:uid="{CC9FF84B-7093-4D0E-ACB8-FDD03E8EF16A}" name="QQ1_CHARACTER_COUNT" dataDxfId="94">
+      <calculatedColumnFormula>LEN(Z2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="29" xr3:uid="{FEE4BCDD-A2C8-4656-9142-5AF890258321}" name="QQ2" dataDxfId="93"/>
+    <tableColumn id="30" xr3:uid="{FF5F779A-A64E-4CB1-B65B-5CA32A55F251}" name="QQ2_CHARACTER_COUNT" dataDxfId="92">
+      <calculatedColumnFormula>LEN(AC2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="31" xr3:uid="{FCAE6D3E-6924-424E-82DC-DA1FD2269340}" name="QQ3" dataDxfId="91"/>
+    <tableColumn id="32" xr3:uid="{ECD1DCF8-19CB-47A7-88FF-807619705842}" name="QQ3_CHARACTER_COUNT" dataDxfId="90">
+      <calculatedColumnFormula>LEN(AE2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="33" xr3:uid="{44BE72B4-0428-49A0-A9B7-BD7E5FEAE33D}" name="QQ3_TYPE_OF_LIE" dataDxfId="89"/>
+    <tableColumn id="34" xr3:uid="{E4BF8E40-1C1A-47FA-9619-D7EB54B8DB08}" name="QQ1 2" dataDxfId="88"/>
+    <tableColumn id="35" xr3:uid="{51242746-597E-450A-8250-ADE59D980592}" name="CHANGED_VIEWS_QQ1" dataDxfId="87"/>
+    <tableColumn id="36" xr3:uid="{5A5B81F5-6563-44EA-8DB7-B9B4ABA28ED3}" name="CHANGED_LENGTH_QQ1" dataDxfId="86"/>
+    <tableColumn id="37" xr3:uid="{46A277CE-6B4C-4496-A820-733A77E959E9}" name="QQ1_CHARACTER_COUNT3" dataDxfId="85">
+      <calculatedColumnFormula>LEN(AH2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="38" xr3:uid="{00A88F16-24F8-49C7-8B6C-BAF6A9A8B609}" name="QQ1_WORD_COUNT_AFTER" dataDxfId="84">
+      <calculatedColumnFormula>IF(LEN(TRIM(AH2))=0, 0, LEN(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(AH2, "/", " "), "-", " "), "  ", " "))) - LEN(SUBSTITUTE(TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(AH2, "/", " "), "-", " "), "  ", " ")), " ", "")) + 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="39" xr3:uid="{D2CFB1E9-9B58-46A4-864B-01E5505E0A24}" name="QQ1_DIFFERENCE_WORD_COUNT" dataDxfId="83">
+      <calculatedColumnFormula>AL2-AA2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="40" xr3:uid="{8C461472-482A-4741-9B6D-5FFFB987CD10}" name="QQ24" dataDxfId="82"/>
+    <tableColumn id="41" xr3:uid="{ACB016F6-819F-41AA-A2F2-D5079B2E9AAC}" name="CHANGED_VIEWS_QQ2" dataDxfId="81"/>
+    <tableColumn id="42" xr3:uid="{3F80A475-1932-4F86-949C-C885FD20CD25}" name="CHANGED_LENGTH_QQ2" dataDxfId="80"/>
+    <tableColumn id="43" xr3:uid="{67924914-4FC3-43C4-B317-D213ED3B7122}" name="QQ2_CHARACTER_COUNT5" dataDxfId="79">
+      <calculatedColumnFormula>LEN(AN2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="44" xr3:uid="{8CD4B191-5EB5-489A-B428-64D7B622CABA}" name="QQ36" dataDxfId="78"/>
+    <tableColumn id="45" xr3:uid="{A3B7A7AD-47E6-41BC-A728-B51182188F6D}" name="QQ3_LIE_2_SUMMARY" dataDxfId="77"/>
+    <tableColumn id="46" xr3:uid="{0AE9B888-FE63-429D-880E-B2FEEA510161}" name="QQ3_CHARACTER_COUNT7" dataDxfId="76">
+      <calculatedColumnFormula>LEN(AR2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="47" xr3:uid="{11CB5346-14BF-4D9F-AAFE-36C0B0FC0B77}" name="QQ1_CHARACTER_COUNT_CHANGE" dataDxfId="75">
+      <calculatedColumnFormula>(AK2-AB2)/AB2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="48" xr3:uid="{2C6DBD2E-6D7F-463F-9E45-C678275E5D7D}" name="QQ2_CHARACTER_COUNT_CHANGE" dataDxfId="74">
+      <calculatedColumnFormula>(AQ2-AD2)/AD2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="49" xr3:uid="{955BA9F3-115D-48D1-8479-E7404B6D4877}" name="QQ3_CHARACTER_COUNT_CHANGE" dataDxfId="73">
+      <calculatedColumnFormula>(AT2-AF2)/AF2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="50" xr3:uid="{52875AA7-BA55-46BB-B509-11A07AE571DF}" name="First Seven Items _1" dataDxfId="72"/>
+    <tableColumn id="51" xr3:uid="{C3E395C6-FA88-421D-964C-A367691119CA}" name="First Seven Items _2" dataDxfId="71"/>
+    <tableColumn id="52" xr3:uid="{57476F5A-91F8-486B-AD0D-CB2878B2596F}" name="First Seven Items _3" dataDxfId="70"/>
+    <tableColumn id="53" xr3:uid="{FFF1781E-3BDD-46F5-BE0D-9907D16FBBB5}" name="First Seven Items _4" dataDxfId="69"/>
+    <tableColumn id="54" xr3:uid="{7D4278ED-E007-413D-910A-5B9118EA06E9}" name="First Seven Items _5" dataDxfId="68"/>
+    <tableColumn id="55" xr3:uid="{5FF1B8E0-11B3-4878-9DE3-C922BE64D779}" name="First Seven Items _6" dataDxfId="67"/>
+    <tableColumn id="56" xr3:uid="{37F27C11-533D-45B1-8485-A661A4070B05}" name="First Seven Items _7" dataDxfId="66"/>
+    <tableColumn id="57" xr3:uid="{9BBED08D-654E-4186-B9E0-02D5BD6DF031}" name="Last Eight Items _1" dataDxfId="65"/>
+    <tableColumn id="58" xr3:uid="{AB5F6026-CE0C-4FBE-B1E4-C0EA0D68AB69}" name="Last Eight Items _2" dataDxfId="64"/>
+    <tableColumn id="59" xr3:uid="{E5777DF9-3867-40CC-9D17-A4BFE08E3385}" name="Last Eight Items _3" dataDxfId="63"/>
+    <tableColumn id="60" xr3:uid="{98A6A1A5-B21D-4EEE-B7F4-28695FDD1EA7}" name="Last Eight Items _4" dataDxfId="62"/>
+    <tableColumn id="61" xr3:uid="{C726EF96-0795-4D73-91D0-0D2DA7E6324D}" name="Last Eight Items _5" dataDxfId="61"/>
+    <tableColumn id="62" xr3:uid="{64DE2DE7-91FC-4CA4-AC29-6ED4D28486EC}" name="Last Eight Items _6" dataDxfId="60"/>
+    <tableColumn id="63" xr3:uid="{EE01A945-CBAC-4806-9223-360E61A55D53}" name="Last Eight Items _7" dataDxfId="59"/>
+    <tableColumn id="64" xr3:uid="{1D250565-C1DC-4501-BA94-F4989086BB47}" name="GCBS PRE SCORE" dataDxfId="58"/>
+    <tableColumn id="65" xr3:uid="{E1DCB0A1-CD04-4844-A1B5-F92862038714}" name="GCBS POST SCORE" dataDxfId="57"/>
+    <tableColumn id="66" xr3:uid="{6F9C5825-9528-4B1E-B5E9-0968FA5F1C59}" name="PRE &amp; POST SCORE" dataDxfId="56">
+      <calculatedColumnFormula>SUM(BL2:BM2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="67" xr3:uid="{64B44018-7B9B-49C9-B47A-10EE07477828}" name="GCBS CHANGE" dataDxfId="55"/>
+    <tableColumn id="68" xr3:uid="{D05EBDF8-6F23-4768-BEC7-290580234D78}" name="First 10 Items _1" dataDxfId="54"/>
+    <tableColumn id="69" xr3:uid="{78FDF35D-A2C9-4F20-ADF1-8F409D16BAC2}" name="First 10 Items _2" dataDxfId="53"/>
+    <tableColumn id="70" xr3:uid="{3849069E-7D74-4A6B-8514-EA1F6C5D9407}" name="First 10 Items _3" dataDxfId="52"/>
+    <tableColumn id="71" xr3:uid="{EB8BD901-B7EE-4753-A93F-7D1B2A8AB05D}" name="First 10 Items _4" dataDxfId="51"/>
+    <tableColumn id="72" xr3:uid="{0B4471B2-A1EC-445E-A221-185AC510DE69}" name="First 10 Items _5" dataDxfId="50"/>
+    <tableColumn id="73" xr3:uid="{A7A45CB3-2699-4173-8356-8CFCC9C26945}" name="First 10 Items _6" dataDxfId="49"/>
+    <tableColumn id="74" xr3:uid="{56639208-C651-4E19-B75F-5BC04D9F277E}" name="First 10 Items _7" dataDxfId="48"/>
+    <tableColumn id="75" xr3:uid="{ED007C6C-8D69-44B2-A49B-6215618A6FF0}" name="First 10 Items _8" dataDxfId="47"/>
+    <tableColumn id="76" xr3:uid="{3D93DA7D-B0AB-4BC3-8323-29758CDC5BF2}" name="First 10 Items _9" dataDxfId="46"/>
+    <tableColumn id="77" xr3:uid="{1BB8D791-37C4-4EC3-9130-1CC37FCB148A}" name="First 10 Items _10" dataDxfId="45"/>
+    <tableColumn id="78" xr3:uid="{0BBACBBC-0134-4580-A6EC-7BD330C8D329}" name="Last 10 Items _1" dataDxfId="44"/>
+    <tableColumn id="79" xr3:uid="{F6B2BFAC-DA1E-4218-8CC4-0C0C543F8F52}" name="Last 10 Items _2" dataDxfId="43"/>
+    <tableColumn id="80" xr3:uid="{40A07F04-9844-4C46-86F1-C428831CCC80}" name="Last 10 Items _3" dataDxfId="42"/>
+    <tableColumn id="81" xr3:uid="{571322F0-B47B-449A-AE94-4457E5840F95}" name="Last 10 Items _4" dataDxfId="41"/>
+    <tableColumn id="82" xr3:uid="{FF7D8433-D3E8-48A2-A2B1-4308E827B752}" name="Last 10 Items _5" dataDxfId="40"/>
+    <tableColumn id="83" xr3:uid="{252891B2-27EE-4339-95DE-2297A9A9A821}" name="Last 10 Items _6" dataDxfId="39"/>
+    <tableColumn id="84" xr3:uid="{5EA6DBB7-21AF-4978-A3FE-EE335C2DB1F8}" name="Last 10 Items _7" dataDxfId="38"/>
+    <tableColumn id="85" xr3:uid="{E735C487-ACBB-404D-A446-33BAC978BC08}" name="Last 10 Items _8" dataDxfId="37"/>
+    <tableColumn id="86" xr3:uid="{F910D3B3-504C-4FBA-9167-582D710FE80D}" name="Last 10 Items _9" dataDxfId="36"/>
+    <tableColumn id="87" xr3:uid="{CB09DEEB-33CA-488F-A988-66B6AFCA2741}" name="Last 10 Items _10" dataDxfId="35"/>
+    <tableColumn id="88" xr3:uid="{A0A76B7C-653F-4BCE-A222-FE7642536DCF}" name="MIST-20 PRE SCORE" dataDxfId="34"/>
+    <tableColumn id="89" xr3:uid="{D7932BF4-CEB8-47A3-A17B-91324F158C4F}" name="MIST-20 POST SCORE" dataDxfId="33"/>
+    <tableColumn id="90" xr3:uid="{9020B670-7601-4440-A455-A98979D9CB17}" name="MIST-20 CHANGE" dataDxfId="32"/>
+    <tableColumn id="91" xr3:uid="{CECB8A50-2F5F-4BAF-8170-D5E92CE3ACAC}" name="First 10 Items _18" dataDxfId="31"/>
+    <tableColumn id="92" xr3:uid="{55EFA626-FDC6-4F77-9551-DB48C565E325}" name="First 10 Items _29" dataDxfId="30"/>
+    <tableColumn id="93" xr3:uid="{D3002C40-62E5-4BDD-AC27-70227AF43CC2}" name="First 10 Items _310" dataDxfId="29"/>
+    <tableColumn id="94" xr3:uid="{4E55AC34-1AED-430E-8A82-86F322574543}" name="First 10 Items _411" dataDxfId="28"/>
+    <tableColumn id="95" xr3:uid="{86F212E2-707D-483A-BE69-EA925F6695A5}" name="First 10 Items _512" dataDxfId="27"/>
+    <tableColumn id="96" xr3:uid="{AD80D84C-8AE1-4AD4-908B-4341AE1BA996}" name="First 10 Items _613" dataDxfId="26"/>
+    <tableColumn id="97" xr3:uid="{7A0331EF-84F9-470D-A941-40A96FFAA5FF}" name="First 10 Items _714" dataDxfId="25"/>
+    <tableColumn id="98" xr3:uid="{E09E2D3C-6845-4205-BF29-282AF853D485}" name="First 10 Items _815" dataDxfId="24"/>
+    <tableColumn id="99" xr3:uid="{AAA88334-9BE2-4DAD-AAFB-A78EF20FB5B8}" name="First 10 Items _916" dataDxfId="23"/>
+    <tableColumn id="100" xr3:uid="{CD64C1BC-E9C3-46BB-B5C5-7614D35C354E}" name="First 10 Items _1017" dataDxfId="22"/>
+    <tableColumn id="101" xr3:uid="{CB8E04AE-7A3E-4496-B191-43B8015D1EA6}" name="Last 10 Items _118" dataDxfId="21"/>
+    <tableColumn id="102" xr3:uid="{C05EA660-6063-4DC8-BDAE-4A69C79843B2}" name="Last 10 Items _219" dataDxfId="20"/>
+    <tableColumn id="103" xr3:uid="{2B0C9DA6-6E2F-4DD8-93FB-C66090EACACA}" name="Last 10 Items _320" dataDxfId="19"/>
+    <tableColumn id="104" xr3:uid="{54652524-2CE9-4BD0-804F-7E97AB0C74F8}" name="Last 10 Items _421" dataDxfId="18"/>
+    <tableColumn id="105" xr3:uid="{6109BB98-1F79-4C5D-BB48-694BE0C63512}" name="Last 10 Items _522" dataDxfId="17"/>
+    <tableColumn id="106" xr3:uid="{054AE5AC-09DB-45C8-90D2-60236DFA98DF}" name="Last 10 Items _623" dataDxfId="16"/>
+    <tableColumn id="107" xr3:uid="{2931BB5E-9A5F-42FC-990B-C0CA7EB4F892}" name="Last 10 Items _724" dataDxfId="15"/>
+    <tableColumn id="108" xr3:uid="{DA38CB37-7A87-47B7-ADC2-CA17CB80D54A}" name="Last 10 Items _825" dataDxfId="14"/>
+    <tableColumn id="109" xr3:uid="{08E9BA4C-8938-4019-BBB8-8A8C7DDB3CA6}" name="Last 10 Items _926" dataDxfId="13"/>
+    <tableColumn id="110" xr3:uid="{546E32DB-1E36-4255-9DF1-028A978E009E}" name="Last 10 Items _1027" dataDxfId="12"/>
+    <tableColumn id="111" xr3:uid="{67BB6F01-8C7D-4B97-9885-C417D3638624}" name="ITMIST PRE SCORE" dataDxfId="11"/>
+    <tableColumn id="112" xr3:uid="{E181337A-2700-48FA-B1EA-C4209E0A7EE3}" name="ITMIST POST SCORE" dataDxfId="10"/>
+    <tableColumn id="113" xr3:uid="{420DFEA7-73B7-484F-89B2-156E45CA05F8}" name="ITMIST CHANGE" dataDxfId="9"/>
+    <tableColumn id="114" xr3:uid="{CC831C4F-FCD4-43DA-8227-B68C9414B21C}" name="1" dataDxfId="8"/>
+    <tableColumn id="115" xr3:uid="{5B964F72-8241-49D4-9725-A6A24FF35745}" name="2" dataDxfId="7"/>
+    <tableColumn id="116" xr3:uid="{8A74599D-823F-46DE-98B0-46B21E30F711}" name="3" dataDxfId="6"/>
+    <tableColumn id="117" xr3:uid="{30DC9047-2565-4B5C-81D2-6E8ADE65B512}" name="4" dataDxfId="5"/>
+    <tableColumn id="118" xr3:uid="{7A310991-FE71-42CD-9CAC-3D74F094CC96}" name="UNDERSTANDABILITY" dataDxfId="4"/>
+    <tableColumn id="119" xr3:uid="{30953372-ED4E-4283-A4F0-0213A7983FD6}" name="SENTIMENT" dataDxfId="3"/>
+    <tableColumn id="120" xr3:uid="{02B27F51-F5A7-4D31-97F0-2F08D06F6140}" name="ADDITIONAL THOUGHTS" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5028,17 +7616,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DP1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" topLeftCell="DH91" workbookViewId="0">
+      <selection activeCell="DO109" sqref="DO109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="16.625" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
     <col min="4" max="4" width="19.125" customWidth="1"/>
-    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="5" max="5" width="12.75" customWidth="1"/>
     <col min="6" max="6" width="34.25" customWidth="1"/>
     <col min="7" max="7" width="38.5" customWidth="1"/>
     <col min="8" max="8" width="23.125" customWidth="1"/>
@@ -5050,17 +7638,14 @@
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="22.75" customWidth="1"/>
     <col min="16" max="16" width="26" customWidth="1"/>
-    <col min="17" max="17" width="22.375" customWidth="1"/>
-    <col min="18" max="19" width="19.75" customWidth="1"/>
-    <col min="20" max="20" width="17.75" customWidth="1"/>
-    <col min="21" max="21" width="19.25" customWidth="1"/>
-    <col min="22" max="22" width="19.625" customWidth="1"/>
+    <col min="17" max="19" width="22.75" customWidth="1"/>
+    <col min="20" max="22" width="21.125" customWidth="1"/>
     <col min="23" max="23" width="22.25" customWidth="1"/>
     <col min="24" max="24" width="20.125" customWidth="1"/>
     <col min="25" max="25" width="20.625" customWidth="1"/>
     <col min="26" max="26" width="46.25" customWidth="1"/>
     <col min="27" max="27" width="33.375" customWidth="1"/>
-    <col min="28" max="28" width="22.625" style="51" customWidth="1"/>
+    <col min="28" max="28" width="27.25" style="51" customWidth="1"/>
     <col min="29" max="29" width="49.75" customWidth="1"/>
     <col min="30" max="30" width="49.75" style="51" customWidth="1"/>
     <col min="31" max="31" width="40.875" customWidth="1"/>
@@ -5068,10 +7653,13 @@
     <col min="33" max="33" width="40.875" customWidth="1"/>
     <col min="34" max="34" width="47.75" customWidth="1"/>
     <col min="35" max="36" width="38.375" customWidth="1"/>
-    <col min="37" max="39" width="27.5" style="47" customWidth="1"/>
+    <col min="37" max="37" width="28.25" style="47" customWidth="1"/>
+    <col min="38" max="38" width="28.625" style="47" customWidth="1"/>
+    <col min="39" max="39" width="34.5" style="47" customWidth="1"/>
     <col min="40" max="43" width="35.125" customWidth="1"/>
     <col min="44" max="45" width="38.375" customWidth="1"/>
-    <col min="46" max="49" width="27.375" style="51" customWidth="1"/>
+    <col min="46" max="46" width="28.25" style="51" customWidth="1"/>
+    <col min="47" max="49" width="36.25" style="51" customWidth="1"/>
     <col min="50" max="63" width="59.75" customWidth="1"/>
     <col min="64" max="64" width="22" style="31" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="23.5" style="31" bestFit="1" customWidth="1"/>
@@ -5079,9 +7667,9 @@
     <col min="67" max="67" width="18.25" style="37" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="59.75" style="33" customWidth="1"/>
     <col min="69" max="87" width="59.75" customWidth="1"/>
-    <col min="88" max="88" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="26.875" customWidth="1"/>
+    <col min="89" max="89" width="28.75" customWidth="1"/>
+    <col min="90" max="90" width="23" customWidth="1"/>
     <col min="91" max="97" width="59.75" customWidth="1"/>
     <col min="98" max="98" width="30.25" customWidth="1"/>
     <col min="99" max="99" width="34.25" customWidth="1"/>
@@ -5096,19 +7684,19 @@
     <col min="108" max="108" width="35.25" customWidth="1"/>
     <col min="109" max="109" width="41.125" customWidth="1"/>
     <col min="110" max="110" width="31.5" customWidth="1"/>
-    <col min="111" max="111" width="14.75" customWidth="1"/>
-    <col min="112" max="112" width="9.25" customWidth="1"/>
-    <col min="113" max="113" width="19.25" customWidth="1"/>
+    <col min="111" max="111" width="25.625" customWidth="1"/>
+    <col min="112" max="112" width="27.5" customWidth="1"/>
+    <col min="113" max="113" width="21.75" customWidth="1"/>
     <col min="114" max="114" width="36.25" style="10" customWidth="1"/>
     <col min="115" max="115" width="24.875" customWidth="1"/>
     <col min="116" max="116" width="31.625" customWidth="1"/>
     <col min="117" max="117" width="23.375" customWidth="1"/>
-    <col min="118" max="118" width="21.75" style="15" customWidth="1"/>
+    <col min="118" max="118" width="23" style="15" customWidth="1"/>
     <col min="119" max="119" width="17.25" style="15" customWidth="1"/>
-    <col min="120" max="120" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" s="10" customFormat="1" ht="72.75" thickBot="1">
+    <row r="1" spans="1:120" s="10" customFormat="1" ht="18.75" thickBot="1">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -5209,7 +7797,7 @@
         <v>1409</v>
       </c>
       <c r="AH1" s="44" t="s">
-        <v>25</v>
+        <v>1420</v>
       </c>
       <c r="AI1" s="44" t="s">
         <v>1400</v>
@@ -5218,7 +7806,7 @@
         <v>1401</v>
       </c>
       <c r="AK1" s="45" t="s">
-        <v>1411</v>
+        <v>1421</v>
       </c>
       <c r="AL1" s="45" t="s">
         <v>1418</v>
@@ -5227,7 +7815,7 @@
         <v>1417</v>
       </c>
       <c r="AN1" s="44" t="s">
-        <v>26</v>
+        <v>1422</v>
       </c>
       <c r="AO1" s="44" t="s">
         <v>1402</v>
@@ -5236,16 +7824,16 @@
         <v>1403</v>
       </c>
       <c r="AQ1" s="45" t="s">
-        <v>1412</v>
+        <v>1423</v>
       </c>
       <c r="AR1" s="44" t="s">
-        <v>27</v>
+        <v>1424</v>
       </c>
       <c r="AS1" s="44" t="s">
         <v>1405</v>
       </c>
       <c r="AT1" s="54" t="s">
-        <v>1413</v>
+        <v>1425</v>
       </c>
       <c r="AU1" s="54" t="s">
         <v>1414</v>
@@ -5380,64 +7968,64 @@
         <v>67</v>
       </c>
       <c r="CM1" s="21" t="s">
-        <v>45</v>
+        <v>1426</v>
       </c>
       <c r="CN1" s="22" t="s">
-        <v>46</v>
+        <v>1427</v>
       </c>
       <c r="CO1" s="22" t="s">
-        <v>47</v>
+        <v>1428</v>
       </c>
       <c r="CP1" s="22" t="s">
-        <v>48</v>
+        <v>1429</v>
       </c>
       <c r="CQ1" s="22" t="s">
-        <v>49</v>
+        <v>1430</v>
       </c>
       <c r="CR1" s="22" t="s">
-        <v>50</v>
+        <v>1431</v>
       </c>
       <c r="CS1" s="22" t="s">
-        <v>51</v>
+        <v>1432</v>
       </c>
       <c r="CT1" s="22" t="s">
-        <v>52</v>
+        <v>1433</v>
       </c>
       <c r="CU1" s="22" t="s">
-        <v>53</v>
+        <v>1434</v>
       </c>
       <c r="CV1" s="23" t="s">
-        <v>54</v>
+        <v>1435</v>
       </c>
       <c r="CW1" s="24" t="s">
-        <v>55</v>
+        <v>1436</v>
       </c>
       <c r="CX1" s="20" t="s">
-        <v>56</v>
+        <v>1437</v>
       </c>
       <c r="CY1" s="20" t="s">
-        <v>57</v>
+        <v>1438</v>
       </c>
       <c r="CZ1" s="20" t="s">
-        <v>58</v>
+        <v>1439</v>
       </c>
       <c r="DA1" s="20" t="s">
-        <v>59</v>
+        <v>1440</v>
       </c>
       <c r="DB1" s="20" t="s">
-        <v>60</v>
+        <v>1441</v>
       </c>
       <c r="DC1" s="20" t="s">
-        <v>61</v>
+        <v>1442</v>
       </c>
       <c r="DD1" s="20" t="s">
-        <v>62</v>
+        <v>1443</v>
       </c>
       <c r="DE1" s="20" t="s">
-        <v>63</v>
+        <v>1444</v>
       </c>
       <c r="DF1" s="25" t="s">
-        <v>64</v>
+        <v>1445</v>
       </c>
       <c r="DG1" s="26" t="s">
         <v>68</v>
@@ -5470,7 +8058,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="2" spans="1:120" ht="200.25">
+    <row r="2" spans="1:120" ht="200.25" hidden="1">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5848,7 +8436,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="3" spans="1:120" ht="43.5">
+    <row r="3" spans="1:120" ht="43.5" hidden="1">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -6226,7 +8814,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:120" ht="43.5">
+    <row r="4" spans="1:120" ht="43.5" hidden="1">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -6604,7 +9192,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="5" spans="1:120" ht="157.5">
+    <row r="5" spans="1:120" ht="157.5" hidden="1">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -6982,7 +9570,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="6" spans="1:120" ht="57.75">
+    <row r="6" spans="1:120" ht="57.75" hidden="1">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -7360,7 +9948,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="7" spans="1:120" ht="143.25">
+    <row r="7" spans="1:120" ht="143.25" hidden="1">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -7738,7 +10326,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="8" spans="1:120" ht="58.5" customHeight="1">
+    <row r="8" spans="1:120" ht="58.5" hidden="1" customHeight="1">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -8116,7 +10704,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="9" spans="1:120" ht="24.75" customHeight="1">
+    <row r="9" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -8494,7 +11082,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="10" spans="1:120" ht="86.25">
+    <row r="10" spans="1:120" ht="86.25" hidden="1">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -8872,7 +11460,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="11" spans="1:120" ht="129">
+    <row r="11" spans="1:120" ht="129" hidden="1">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -9250,7 +11838,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="12" spans="1:120" ht="43.5">
+    <row r="12" spans="1:120" ht="43.5" hidden="1">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -9628,7 +12216,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="13" spans="1:120" ht="57.75">
+    <row r="13" spans="1:120" ht="57.75" hidden="1">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -10006,7 +12594,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="14" spans="1:120" ht="143.25">
+    <row r="14" spans="1:120" ht="143.25" hidden="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -10384,7 +12972,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:120" ht="100.5">
+    <row r="15" spans="1:120" ht="100.5" hidden="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -10762,7 +13350,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="16" spans="1:120" ht="57.75">
+    <row r="16" spans="1:120" ht="57.75" hidden="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -11140,7 +13728,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="17" spans="1:120" ht="105.75" customHeight="1">
+    <row r="17" spans="1:120" ht="105.75" hidden="1" customHeight="1">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -11518,7 +14106,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="18" spans="1:120" ht="127.5" customHeight="1">
+    <row r="18" spans="1:120" ht="127.5" hidden="1" customHeight="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -12274,7 +14862,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="20" spans="1:120" ht="67.900000000000006" customHeight="1">
+    <row r="20" spans="1:120" ht="67.900000000000006" hidden="1" customHeight="1">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12652,7 +15240,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="21" spans="1:120" ht="72">
+    <row r="21" spans="1:120" ht="72" hidden="1">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -13030,7 +15618,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="22" spans="1:120" ht="114.75">
+    <row r="22" spans="1:120" ht="114.75" hidden="1">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13408,7 +15996,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="23" spans="1:120" ht="86.25">
+    <row r="23" spans="1:120" ht="86.25" hidden="1">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -14920,7 +17508,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="27" spans="1:120" ht="57.75">
+    <row r="27" spans="1:120" ht="57.75" hidden="1">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -15298,7 +17886,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="28" spans="1:120" ht="100.5">
+    <row r="28" spans="1:120" ht="100.5" hidden="1">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -16054,7 +18642,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="30" spans="1:120" ht="114.75">
+    <row r="30" spans="1:120" ht="114.75" hidden="1">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -16432,7 +19020,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="31" spans="1:120" ht="86.25">
+    <row r="31" spans="1:120" ht="86.25" hidden="1">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -16810,7 +19398,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="32" spans="1:120" ht="43.5">
+    <row r="32" spans="1:120" ht="43.5" hidden="1">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -17188,7 +19776,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="33" spans="1:120" ht="129">
+    <row r="33" spans="1:120" ht="129" hidden="1">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -17566,7 +20154,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="34" spans="1:120" ht="72">
+    <row r="34" spans="1:120" ht="72" hidden="1">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -17944,7 +20532,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="35" spans="1:120" ht="43.5">
+    <row r="35" spans="1:120" ht="43.5" hidden="1">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -18322,7 +20910,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="36" spans="1:120" ht="86.25">
+    <row r="36" spans="1:120" ht="86.25" hidden="1">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -18700,7 +21288,7 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="37" spans="1:120" ht="43.5">
+    <row r="37" spans="1:120" ht="43.5" hidden="1">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -19456,7 +22044,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="39" spans="1:120" ht="24.75" customHeight="1">
+    <row r="39" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -19834,7 +22422,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="40" spans="1:120" ht="100.5">
+    <row r="40" spans="1:120" ht="100.5" hidden="1">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -20212,7 +22800,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="41" spans="1:120" ht="98.25" customHeight="1">
+    <row r="41" spans="1:120" ht="98.25" hidden="1" customHeight="1">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -20590,7 +23178,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="42" spans="1:120" ht="145.5" customHeight="1">
+    <row r="42" spans="1:120" ht="145.5" hidden="1" customHeight="1">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -20968,7 +23556,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="43" spans="1:120" ht="249" customHeight="1">
+    <row r="43" spans="1:120" ht="249" hidden="1" customHeight="1">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -21720,7 +24308,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="45" spans="1:120" ht="86.25">
+    <row r="45" spans="1:120" ht="86.25" hidden="1">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -22098,7 +24686,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="46" spans="1:120" ht="24.75" customHeight="1">
+    <row r="46" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -22476,7 +25064,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="47" spans="1:120" ht="75" customHeight="1">
+    <row r="47" spans="1:120" ht="75" hidden="1" customHeight="1">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -22854,7 +25442,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="48" spans="1:120" ht="129">
+    <row r="48" spans="1:120" ht="129" hidden="1">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -23232,7 +25820,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="49" spans="1:120" ht="72">
+    <row r="49" spans="1:120" ht="72" hidden="1">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -23610,7 +26198,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="50" spans="1:120" ht="105" customHeight="1">
+    <row r="50" spans="1:120" ht="105" hidden="1" customHeight="1">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -23988,7 +26576,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="51" spans="1:120" ht="113.25" customHeight="1">
+    <row r="51" spans="1:120" ht="113.25" hidden="1" customHeight="1">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -24366,7 +26954,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="52" spans="1:120" ht="66" customHeight="1">
+    <row r="52" spans="1:120" ht="66" hidden="1" customHeight="1">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -24744,7 +27332,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="53" spans="1:120" ht="59.45" customHeight="1">
+    <row r="53" spans="1:120" ht="59.45" hidden="1" customHeight="1">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -25122,7 +27710,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="54" spans="1:120" ht="129">
+    <row r="54" spans="1:120" ht="129" hidden="1">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -25500,7 +28088,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="55" spans="1:120" ht="24.75" customHeight="1">
+    <row r="55" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -25878,7 +28466,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="56" spans="1:120" ht="91.5" customHeight="1">
+    <row r="56" spans="1:120" ht="91.5" hidden="1" customHeight="1">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -26256,7 +28844,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="57" spans="1:120" ht="114.75">
+    <row r="57" spans="1:120" ht="114.75" hidden="1">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -26634,7 +29222,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="58" spans="1:120" ht="24.75" customHeight="1">
+    <row r="58" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -27012,7 +29600,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="59" spans="1:120" ht="100.5">
+    <row r="59" spans="1:120" ht="100.5" hidden="1">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -27390,7 +29978,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="60" spans="1:120" ht="29.25">
+    <row r="60" spans="1:120" ht="29.25" hidden="1">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -27768,7 +30356,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="61" spans="1:120" ht="72">
+    <row r="61" spans="1:120" ht="72" hidden="1">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -28902,7 +31490,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="64" spans="1:120" ht="169.9" customHeight="1">
+    <row r="64" spans="1:120" ht="169.9" hidden="1" customHeight="1">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -30036,7 +32624,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="67" spans="1:120" ht="43.15" customHeight="1">
+    <row r="67" spans="1:120" ht="43.15" hidden="1" customHeight="1">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -30792,7 +33380,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="69" spans="1:120" ht="143.25">
+    <row r="69" spans="1:120" ht="143.25" hidden="1">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -31548,7 +34136,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="71" spans="1:120" ht="138" customHeight="1">
+    <row r="71" spans="1:120" ht="138" hidden="1" customHeight="1">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -31926,7 +34514,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="72" spans="1:120" ht="112.5" customHeight="1">
+    <row r="72" spans="1:120" ht="112.5" hidden="1" customHeight="1">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -32304,7 +34892,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="73" spans="1:120" ht="157.15" customHeight="1">
+    <row r="73" spans="1:120" ht="157.15" hidden="1" customHeight="1">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -32682,7 +35270,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="74" spans="1:120" ht="43.5">
+    <row r="74" spans="1:120" ht="43.5" hidden="1">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -33060,7 +35648,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="75" spans="1:120" ht="142.5" customHeight="1">
+    <row r="75" spans="1:120" ht="142.5" hidden="1" customHeight="1">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -33438,7 +36026,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="76" spans="1:120" ht="43.9" customHeight="1">
+    <row r="76" spans="1:120" ht="43.9" hidden="1" customHeight="1">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -33816,7 +36404,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="77" spans="1:120" ht="87.6" customHeight="1">
+    <row r="77" spans="1:120" ht="87.6" hidden="1" customHeight="1">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -34194,7 +36782,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="78" spans="1:120" ht="33" customHeight="1">
+    <row r="78" spans="1:120" ht="33" hidden="1" customHeight="1">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -34572,7 +37160,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="79" spans="1:120" ht="54.6" customHeight="1">
+    <row r="79" spans="1:120" ht="54.6" hidden="1" customHeight="1">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -35328,7 +37916,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="81" spans="1:120" ht="64.150000000000006" customHeight="1">
+    <row r="81" spans="1:120" ht="64.150000000000006" hidden="1" customHeight="1">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -35706,7 +38294,7 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="82" spans="1:120" ht="75" customHeight="1">
+    <row r="82" spans="1:120" ht="75" hidden="1" customHeight="1">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -36840,7 +39428,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="85" spans="1:120" ht="75" customHeight="1">
+    <row r="85" spans="1:120" ht="75" hidden="1" customHeight="1">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -37218,7 +39806,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="86" spans="1:120" ht="53.45" customHeight="1">
+    <row r="86" spans="1:120" ht="53.45" hidden="1" customHeight="1">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -37596,7 +40184,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="87" spans="1:120" ht="141.75" customHeight="1">
+    <row r="87" spans="1:120" ht="141.75" hidden="1" customHeight="1">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -38352,7 +40940,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="89" spans="1:120" ht="97.9" customHeight="1">
+    <row r="89" spans="1:120" ht="97.9" hidden="1" customHeight="1">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -39486,7 +42074,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="92" spans="1:120" ht="245.25" customHeight="1">
+    <row r="92" spans="1:120" ht="245.25" hidden="1" customHeight="1">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -39864,7 +42452,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="93" spans="1:120" ht="43.9" customHeight="1">
+    <row r="93" spans="1:120" ht="43.9" hidden="1" customHeight="1">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -40242,7 +42830,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="94" spans="1:120" ht="53.45" customHeight="1">
+    <row r="94" spans="1:120" ht="53.45" hidden="1" customHeight="1">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -40998,7 +43586,7 @@
         <v>1379</v>
       </c>
     </row>
-    <row r="96" spans="1:120" ht="43.9" customHeight="1">
+    <row r="96" spans="1:120" ht="43.9" hidden="1" customHeight="1">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -41754,7 +44342,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="98" spans="1:120" ht="86.25">
+    <row r="98" spans="1:120" ht="86.25" hidden="1">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -42132,7 +44720,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="99" spans="1:120" ht="231" customHeight="1">
+    <row r="99" spans="1:120" ht="231" hidden="1" customHeight="1">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -42510,7 +45098,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="100" spans="1:120" ht="120" customHeight="1">
+    <row r="100" spans="1:120" ht="120" hidden="1" customHeight="1">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -42888,7 +45476,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="101" spans="1:120" ht="24.75" customHeight="1">
+    <row r="101" spans="1:120" ht="24.75" hidden="1" customHeight="1">
       <c r="AA101" s="55">
         <f t="shared" si="20"/>
         <v>0</v>
@@ -52011,5 +54599,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
analysis for future study
</commit_message>
<xml_diff>
--- a/analysis/data/lying_data.xlsx
+++ b/analysis/data/lying_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\School\2025\Spring 2025\INFO 698 - Capstone\GitHub Repo\misinformation-study\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FDB35-5D7B-4929-AF92-3FD88FBB42AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4089ACD-A24C-4FDD-95E9-DCF4D1338E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7731,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DR1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CV1" workbookViewId="0">
-      <selection activeCell="DB3" sqref="DB3"/>
+    <sheetView tabSelected="1" topLeftCell="X4" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -56735,7 +56735,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU19:AU100 AU2:AU17 AN3:AN100 AL2:AL100" xr:uid="{5FBD5AA7-16D2-437E-B72E-9EF6476D3ACD}">
       <formula1>"View stayed about the same, View had some/moderate change, View significantantly changed"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
added new poster templates & examples
</commit_message>
<xml_diff>
--- a/analysis/data/lying_data.xlsx
+++ b/analysis/data/lying_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\School\2025\Spring 2025\INFO 698 - Capstone\GitHub Repo\misinformation-study\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4089ACD-A24C-4FDD-95E9-DCF4D1338E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557616CB-16C3-4AAD-BFA7-BEF198D0C9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7731,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DR1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X4" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>